<commit_message>
Add feedbacked on deliverables
</commit_message>
<xml_diff>
--- a/Oswyn/Feedback.xlsx
+++ b/Oswyn/Feedback.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
   <si>
     <t>Author</t>
   </si>
@@ -131,6 +131,91 @@
   <si>
     <t>Update with the process you go through to complete a task assigned to you. See the Work Process Presentation for a starting point</t>
   </si>
+  <si>
+    <t>a8c6fd6</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">" DEFINED AREA FOR DRAWING AN ARC." this is a good product level characteristics. But how big is the drawing area specifcially </t>
+  </si>
+  <si>
+    <t>Add dimensions of drawing area</t>
+  </si>
+  <si>
+    <t>Poduct Characteristics</t>
+  </si>
+  <si>
+    <t>This is also the place to say that this is for making post cards</t>
+  </si>
+  <si>
+    <t>"- DSP FOR PRECISE MOTOR MOVEMENTS
+ - EMBEDDED CODE FOR OPERATING LOGIC" these associated with features not the whole product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move them to the feature associated with them. </t>
+  </si>
+  <si>
+    <t>AUDRIO</t>
+  </si>
+  <si>
+    <t>spelling</t>
+  </si>
+  <si>
+    <t>General Chacteristics</t>
+  </si>
+  <si>
+    <t>Thre are some general issues we should go over abou this</t>
+  </si>
+  <si>
+    <t>Lets set up a call to go through it</t>
+  </si>
+  <si>
+    <t>General Behavior</t>
+  </si>
+  <si>
+    <t>Major Components BOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULN2003 is the part number not the module number. </t>
+  </si>
+  <si>
+    <t>If you gave this number to someone they would order the wrong thing. Update the Vendor and Vendor part number with the module you actually want to buy</t>
+  </si>
+  <si>
+    <t>Joystick breakout board module does not have a part number</t>
+  </si>
+  <si>
+    <t>I need a part number to buy against so you need to include one</t>
+  </si>
+  <si>
+    <t>"Collision sensor limit switch module " no vendor part number</t>
+  </si>
+  <si>
+    <t>Add a part number</t>
+  </si>
+  <si>
+    <t>You need to add the mechanical parts to your Feature List</t>
+  </si>
+  <si>
+    <t>Add the arms but mark them as mechaical components</t>
+  </si>
+  <si>
+    <t>Feature List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General </t>
+  </si>
+  <si>
+    <t>Try and limit the number of places order from</t>
+  </si>
+  <si>
+    <t>Sub-funcation parts set not marked</t>
+  </si>
+  <si>
+    <t>I need to know what subset of parts I need to buy so mark them somehow</t>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,16 +277,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -209,8 +315,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -264,8 +379,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -296,8 +449,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -324,6 +488,25 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -350,6 +533,25 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -679,241 +881,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="9" customWidth="1"/>
-    <col min="4" max="4" width="55" style="10" customWidth="1"/>
-    <col min="5" max="5" width="66.5" style="10" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55" style="10" customWidth="1"/>
+    <col min="6" max="6" width="66.5" style="10" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="G2" s="2"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="G3" s="2"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="G4" s="2"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="6"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="G5" s="2"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="48">
+    <row r="7" spans="1:9" ht="48">
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="48">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="48">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="E8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="48">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="48">
-      <c r="A9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="E10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="E11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="80">
+      <c r="A12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="80">
-      <c r="A12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="E12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="48">
+      <c r="A13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="48">
-      <c r="A13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="E13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="32">
+      <c r="A14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="32">
-      <c r="A14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="E14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="32">
+      <c r="A15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="32">
-      <c r="A15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="14" customFormat="1">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" ht="48">
+      <c r="A17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="48">
+      <c r="A19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="48">
+      <c r="A24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="32">
+      <c r="A26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="E28" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>